<commit_message>
Updating README.md in assembly folder.
</commit_message>
<xml_diff>
--- a/assembly/bom-bluetooth-tracker.xlsx
+++ b/assembly/bom-bluetooth-tracker.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewli/Documents/Andrew/Archive/Scratch/Garage Projects/Electronics Projects/Bluetooth Tracker/bluetooth-tracker/assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B11199F3-1415-974C-8D27-82BF669DDFC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A57390A-35DF-4C4E-924F-7B6978CF5072}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bluetooth-tracker" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t>Reference</t>
   </si>
@@ -178,9 +178,6 @@
     <t xml:space="preserve">Q1 </t>
   </si>
   <si>
-    <t>FDV301N_G</t>
-  </si>
-  <si>
     <t>MOSFET N-CH 25V 220MA SOT-23</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t xml:space="preserve">R2 </t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
     <t>RES SMD 100K OHM 1% 1/16W 0402</t>
   </si>
   <si>
@@ -208,9 +202,6 @@
     <t xml:space="preserve">R3 R1 </t>
   </si>
   <si>
-    <t>1k</t>
-  </si>
-  <si>
     <t>RES SMD 1K OHM 1% 1/16W 0402</t>
   </si>
   <si>
@@ -220,9 +211,6 @@
     <t xml:space="preserve">U1 </t>
   </si>
   <si>
-    <t>NRF51822-QFAA-T_G</t>
-  </si>
-  <si>
     <t>IC RF TXRX+MCU BLUETOOTH 48VFQFN</t>
   </si>
   <si>
@@ -235,9 +223,6 @@
     <t xml:space="preserve">XTAL1 </t>
   </si>
   <si>
-    <t>ECS-_327-12_5-34B-TR</t>
-  </si>
-  <si>
     <t>CRYSTAL 32.7680KHZ 12.5PF SMD</t>
   </si>
   <si>
@@ -257,12 +242,18 @@
   </si>
   <si>
     <t>NDK America, Inc.</t>
+  </si>
+  <si>
+    <t>100kΩ</t>
+  </si>
+  <si>
+    <t>1kΩ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1102,10 +1093,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1136,7 +1129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1156,7 +1149,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1176,7 +1169,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1189,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1216,7 +1209,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1236,7 +1229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1256,7 +1249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -1276,7 +1269,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -1296,7 +1289,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
@@ -1316,7 +1309,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -1336,7 +1329,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -1356,7 +1349,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1364,116 +1357,116 @@
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>